<commit_message>
Update cognito_users.py according to new Excel format
</commit_message>
<xml_diff>
--- a/awscognito/sample.xlsx
+++ b/awscognito/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckwu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3163EF3-9AB7-460B-8D2A-282078B14371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D9F11F-3C4C-4416-9F79-232B230F3878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -20,85 +20,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>middle_name</t>
-  </si>
-  <si>
-    <t>preferred_name</t>
-  </si>
-  <si>
-    <t>affiliation</t>
-  </si>
-  <si>
-    <t>timezone</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>a_last</t>
+    <t>name</t>
   </si>
   <si>
-    <t>a_first</t>
+    <t>committee</t>
   </si>
   <si>
-    <t>a_middle</t>
+    <t>jane.doe@gmail.com</t>
   </si>
   <si>
-    <t>a</t>
+    <t>john.deo@gmail.com</t>
   </si>
   <si>
-    <t>a_company</t>
+    <t>Jane Doe</t>
   </si>
   <si>
-    <t>Asia/Hong_Kong</t>
+    <t>John Doe</t>
   </si>
   <si>
-    <t>Hong Kong</t>
+    <t>Virtual Infrastructure</t>
   </si>
   <si>
-    <t>example+a@gmail.com</t>
-  </si>
-  <si>
-    <t>b_last</t>
-  </si>
-  <si>
-    <t>b_first</t>
-  </si>
-  <si>
-    <t>b_middle</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>b_company</t>
-  </si>
-  <si>
-    <t>Asia/Seoul</t>
-  </si>
-  <si>
-    <t>Korea</t>
-  </si>
-  <si>
-    <t>example+b@gmail.com</t>
+    <t>Tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +184,24 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -574,11 +547,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -612,10 +591,12 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{8133163B-20C5-426A-A3D2-D72F36B58DA3}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -932,91 +913,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F6B9B003-F4F6-42FC-842F-9D50830758F1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4BEE77C7-C914-4E14-87AB-4774B6E1BE54}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>